<commit_message>
Menejo de la matriz con exel
</commit_message>
<xml_diff>
--- a/TRAND.xlsx
+++ b/TRAND.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hevi-\Desktop\Lenguajes y automatas I\Lexico_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32907E60-9D87-4589-88DD-465902453F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4302CD9-FC1A-4029-ACD9-C4FC3B447167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B55FBFE-415A-4501-9873-421BD18FE1C4}"/>
+    <workbookView xWindow="7005" yWindow="765" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{0B55FBFE-415A-4501-9873-421BD18FE1C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="28">
   <si>
     <t>WS</t>
   </si>
@@ -186,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +215,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCB97DA-E567-4BFA-BCA5-8FB704E652E1}">
   <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="136" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -3877,4 +3881,3059 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27552F2-8742-4294-B48A-0D8C8D469A6B}">
+  <dimension ref="A1:Z38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1">
+        <v>25</v>
+      </c>
+      <c r="T1" s="1">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1">
+        <v>29</v>
+      </c>
+      <c r="V1" s="1">
+        <v>32</v>
+      </c>
+      <c r="W1" s="1">
+        <v>34</v>
+      </c>
+      <c r="X1" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="15">
+      <c r="A2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15">
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15">
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1">
+        <v>13</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="1">
+        <v>13</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15">
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1">
+        <v>13</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="1">
+        <v>13</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S15" s="1">
+        <v>15</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="15">
+      <c r="A17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="1">
+        <v>17</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="15">
+      <c r="A18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="15">
+      <c r="A19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O19" s="1">
+        <v>19</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15">
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="15">
+      <c r="A21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" s="8">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z21" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15">
+      <c r="A22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="8">
+        <v>22</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z22" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="15">
+      <c r="A23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z23" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="15">
+      <c r="A24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" s="8">
+        <v>24</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z24" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="15">
+      <c r="A25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z25" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="15">
+      <c r="A26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="5">
+        <v>24</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z26" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="15">
+      <c r="A27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="5">
+        <v>24</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S27" s="5">
+        <v>24</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z27" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="15">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5">
+        <v>27</v>
+      </c>
+      <c r="E28" s="5">
+        <v>27</v>
+      </c>
+      <c r="F28" s="5">
+        <v>27</v>
+      </c>
+      <c r="G28" s="5">
+        <v>27</v>
+      </c>
+      <c r="H28" s="5">
+        <v>27</v>
+      </c>
+      <c r="I28" s="5">
+        <v>27</v>
+      </c>
+      <c r="J28" s="5">
+        <v>27</v>
+      </c>
+      <c r="K28" s="5">
+        <v>27</v>
+      </c>
+      <c r="L28" s="5">
+        <v>27</v>
+      </c>
+      <c r="M28" s="5">
+        <v>27</v>
+      </c>
+      <c r="N28" s="5">
+        <v>27</v>
+      </c>
+      <c r="O28" s="5">
+        <v>27</v>
+      </c>
+      <c r="P28" s="5">
+        <v>27</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>27</v>
+      </c>
+      <c r="R28" s="5">
+        <v>27</v>
+      </c>
+      <c r="S28" s="5">
+        <v>27</v>
+      </c>
+      <c r="T28" s="5">
+        <v>28</v>
+      </c>
+      <c r="U28" s="5">
+        <v>27</v>
+      </c>
+      <c r="V28" s="5">
+        <v>27</v>
+      </c>
+      <c r="W28" s="5">
+        <v>27</v>
+      </c>
+      <c r="X28" s="5">
+        <v>27</v>
+      </c>
+      <c r="Y28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z28" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="15">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z29" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="A30" s="5">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5">
+        <v>30</v>
+      </c>
+      <c r="C30" s="5">
+        <v>30</v>
+      </c>
+      <c r="D30" s="5">
+        <v>30</v>
+      </c>
+      <c r="E30" s="5">
+        <v>30</v>
+      </c>
+      <c r="F30" s="5">
+        <v>30</v>
+      </c>
+      <c r="G30" s="5">
+        <v>30</v>
+      </c>
+      <c r="H30" s="5">
+        <v>30</v>
+      </c>
+      <c r="I30" s="5">
+        <v>30</v>
+      </c>
+      <c r="J30" s="5">
+        <v>30</v>
+      </c>
+      <c r="K30" s="5">
+        <v>30</v>
+      </c>
+      <c r="L30" s="5">
+        <v>30</v>
+      </c>
+      <c r="M30" s="5">
+        <v>30</v>
+      </c>
+      <c r="N30" s="5">
+        <v>30</v>
+      </c>
+      <c r="O30" s="5">
+        <v>30</v>
+      </c>
+      <c r="P30" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>30</v>
+      </c>
+      <c r="R30" s="5">
+        <v>30</v>
+      </c>
+      <c r="S30" s="5">
+        <v>30</v>
+      </c>
+      <c r="T30" s="5">
+        <v>30</v>
+      </c>
+      <c r="U30" s="5">
+        <v>30</v>
+      </c>
+      <c r="V30" s="5">
+        <v>30</v>
+      </c>
+      <c r="W30" s="5">
+        <v>30</v>
+      </c>
+      <c r="X30" s="5">
+        <v>30</v>
+      </c>
+      <c r="Y30" s="5">
+        <v>30</v>
+      </c>
+      <c r="Z30" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="15">
+      <c r="A31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U31" s="5">
+        <v>31</v>
+      </c>
+      <c r="V31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="W31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z31" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="15">
+      <c r="A32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z32" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="15">
+      <c r="A33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="5">
+        <v>32</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z33" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="15">
+      <c r="A34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z34" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="15">
+      <c r="A35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" s="5">
+        <v>17</v>
+      </c>
+      <c r="M35" s="5">
+        <v>36</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W35" s="5">
+        <v>35</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z35" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5">
+        <v>35</v>
+      </c>
+      <c r="C36" s="5">
+        <v>35</v>
+      </c>
+      <c r="D36" s="5">
+        <v>35</v>
+      </c>
+      <c r="E36" s="5">
+        <v>35</v>
+      </c>
+      <c r="F36" s="5">
+        <v>35</v>
+      </c>
+      <c r="G36" s="5">
+        <v>35</v>
+      </c>
+      <c r="H36" s="5">
+        <v>35</v>
+      </c>
+      <c r="I36" s="5">
+        <v>35</v>
+      </c>
+      <c r="J36" s="5">
+        <v>35</v>
+      </c>
+      <c r="K36" s="5">
+        <v>35</v>
+      </c>
+      <c r="L36" s="5">
+        <v>35</v>
+      </c>
+      <c r="M36" s="5">
+        <v>35</v>
+      </c>
+      <c r="N36" s="5">
+        <v>35</v>
+      </c>
+      <c r="O36" s="5">
+        <v>35</v>
+      </c>
+      <c r="P36" s="5">
+        <v>35</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>35</v>
+      </c>
+      <c r="R36" s="5">
+        <v>35</v>
+      </c>
+      <c r="S36" s="5">
+        <v>35</v>
+      </c>
+      <c r="T36" s="5">
+        <v>35</v>
+      </c>
+      <c r="U36" s="5">
+        <v>35</v>
+      </c>
+      <c r="V36" s="5">
+        <v>35</v>
+      </c>
+      <c r="W36" s="5">
+        <v>35</v>
+      </c>
+      <c r="X36" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="5">
+        <v>35</v>
+      </c>
+      <c r="Z36" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5">
+        <v>36</v>
+      </c>
+      <c r="C37" s="5">
+        <v>36</v>
+      </c>
+      <c r="D37" s="5">
+        <v>36</v>
+      </c>
+      <c r="E37" s="5">
+        <v>36</v>
+      </c>
+      <c r="F37" s="5">
+        <v>36</v>
+      </c>
+      <c r="G37" s="5">
+        <v>36</v>
+      </c>
+      <c r="H37" s="5">
+        <v>36</v>
+      </c>
+      <c r="I37" s="5">
+        <v>36</v>
+      </c>
+      <c r="J37" s="5">
+        <v>36</v>
+      </c>
+      <c r="K37" s="5">
+        <v>36</v>
+      </c>
+      <c r="L37" s="5">
+        <v>36</v>
+      </c>
+      <c r="M37" s="5">
+        <v>37</v>
+      </c>
+      <c r="N37" s="5">
+        <v>36</v>
+      </c>
+      <c r="O37" s="5">
+        <v>36</v>
+      </c>
+      <c r="P37" s="5">
+        <v>36</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>36</v>
+      </c>
+      <c r="R37" s="5">
+        <v>36</v>
+      </c>
+      <c r="S37" s="5">
+        <v>36</v>
+      </c>
+      <c r="T37" s="5">
+        <v>36</v>
+      </c>
+      <c r="U37" s="5">
+        <v>36</v>
+      </c>
+      <c r="V37" s="5">
+        <v>36</v>
+      </c>
+      <c r="W37" s="5">
+        <v>36</v>
+      </c>
+      <c r="X37" s="5">
+        <v>36</v>
+      </c>
+      <c r="Y37" s="5">
+        <v>36</v>
+      </c>
+      <c r="Z37" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26">
+      <c r="A38" s="5">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <v>36</v>
+      </c>
+      <c r="C38" s="5">
+        <v>36</v>
+      </c>
+      <c r="D38" s="5">
+        <v>36</v>
+      </c>
+      <c r="E38" s="5">
+        <v>36</v>
+      </c>
+      <c r="F38" s="5">
+        <v>36</v>
+      </c>
+      <c r="G38" s="5">
+        <v>36</v>
+      </c>
+      <c r="H38" s="5">
+        <v>36</v>
+      </c>
+      <c r="I38" s="5">
+        <v>36</v>
+      </c>
+      <c r="J38" s="5">
+        <v>36</v>
+      </c>
+      <c r="K38" s="5">
+        <v>36</v>
+      </c>
+      <c r="L38" s="5">
+        <v>36</v>
+      </c>
+      <c r="M38" s="5">
+        <v>37</v>
+      </c>
+      <c r="N38" s="5">
+        <v>36</v>
+      </c>
+      <c r="O38" s="5">
+        <v>36</v>
+      </c>
+      <c r="P38" s="5">
+        <v>36</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>36</v>
+      </c>
+      <c r="R38" s="5">
+        <v>36</v>
+      </c>
+      <c r="S38" s="5">
+        <v>36</v>
+      </c>
+      <c r="T38" s="5">
+        <v>36</v>
+      </c>
+      <c r="U38" s="5">
+        <v>36</v>
+      </c>
+      <c r="V38" s="5">
+        <v>36</v>
+      </c>
+      <c r="W38" s="5">
+        <v>0</v>
+      </c>
+      <c r="X38" s="5">
+        <v>36</v>
+      </c>
+      <c r="Y38" s="5">
+        <v>36</v>
+      </c>
+      <c r="Z38" s="5">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>